<commit_message>
Added coil temps csv files, coil temp script, man_phant_vids
</commit_message>
<xml_diff>
--- a/data/cadaver/AID.xlsx
+++ b/data/cadaver/AID.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>Manual</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Avg Increase in EA AID</t>
+  </si>
+  <si>
+    <t>STD</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -188,14 +191,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +485,7 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -492,27 +498,27 @@
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
@@ -766,7 +772,7 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="1"/>
@@ -778,7 +784,7 @@
       <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="1"/>
@@ -793,29 +799,29 @@
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="9" t="s">
+      <c r="D14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -852,6 +858,9 @@
       <c r="L15" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="M15" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="R15" s="2"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -894,6 +903,10 @@
         <f>AVERAGE(I16:K16)</f>
         <v>479.33333333333331</v>
       </c>
+      <c r="M16" s="11">
+        <f>_xlfn.STDEV.S(I16:K16)</f>
+        <v>35.851545759330008</v>
+      </c>
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -936,6 +949,10 @@
         <f t="shared" ref="L17:L18" si="2">AVERAGE(I17:K17)</f>
         <v>437</v>
       </c>
+      <c r="M17" s="11">
+        <f t="shared" ref="M17:M18" si="3">_xlfn.STDEV.S(I17:K17)</f>
+        <v>59.908263203000637</v>
+      </c>
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -978,6 +995,10 @@
         <f t="shared" si="2"/>
         <v>459</v>
       </c>
+      <c r="M18" s="11">
+        <f t="shared" si="3"/>
+        <v>135.5249054602142</v>
+      </c>
       <c r="R18" s="2"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -1089,7 +1110,7 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="F24" s="10">
+      <c r="F24" s="9">
         <f>AVERAGE(F15:F17)</f>
         <v>12.666666666666666</v>
       </c>
@@ -1098,7 +1119,7 @@
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="F25" s="10">
+      <c r="F25" s="9">
         <f>AVERAGE(F18:F23)</f>
         <v>56.833333333333336</v>
       </c>

</xml_diff>